<commit_message>
Updated, more de-idenitfied profiles
</commit_message>
<xml_diff>
--- a/raw-data/table.xlsx
+++ b/raw-data/table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dshap\Documents\GOV-1006\Table\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dshap\Documents\GOV-1006\thesis_prep\raw-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC809954-7315-4267-A16C-65B2CC0AAF67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B57C57F-2DAB-4EA0-813F-2D263C7208E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FF94495B-E4B7-491F-A458-C863B44AD365}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
   <si>
     <t>Vladimir</t>
   </si>
@@ -120,27 +120,6 @@
   </si>
   <si>
     <t>No</t>
-  </si>
-  <si>
-    <t>Yes, California</t>
-  </si>
-  <si>
-    <t>Yes, studied in California</t>
-  </si>
-  <si>
-    <t>Yes, studied in New York, interned in California, been to Washington D.C., Atlanta, Boston</t>
-  </si>
-  <si>
-    <t>Yes, New York, Boston, D.C.</t>
-  </si>
-  <si>
-    <t>Yes, New York</t>
-  </si>
-  <si>
-    <t>Yes, New York, Boston</t>
-  </si>
-  <si>
-    <t>Yes, upstate New York and most of the Northeast</t>
   </si>
   <si>
     <t>Yes</t>
@@ -524,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF9EBBB9-54FD-4869-9E1B-3DF0F6D23EB8}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -538,19 +517,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
@@ -567,7 +546,7 @@
         <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -581,10 +560,10 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -601,7 +580,7 @@
         <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -618,7 +597,7 @@
         <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -632,10 +611,10 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -652,7 +631,7 @@
         <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -666,10 +645,10 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -703,7 +682,7 @@
         <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -717,10 +696,10 @@
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -734,10 +713,10 @@
         <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -754,7 +733,7 @@
         <v>28</v>
       </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -768,10 +747,10 @@
         <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -788,7 +767,7 @@
         <v>28</v>
       </c>
       <c r="E15" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>